<commit_message>
Atualização de comentários do código
Code comments update
</commit_message>
<xml_diff>
--- a/colaboradores.xlsx
+++ b/colaboradores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\GitHub\esocial\esocial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28075D6B-1D91-4AF1-87E9-BCA6AEDA074A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD55602-535D-4F7D-BD9E-D1298B0D2DF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -466,17 +466,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB3"/>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X13" sqref="X13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -570,11 +568,6 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>987654321</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>